<commit_message>
Moving the ShoppersStack project to GitHub
</commit_message>
<xml_diff>
--- a/ShopperStack_QUKN1/src/test/resources/TestData/ExcelFile.xlsx
+++ b/ShopperStack_QUKN1/src/test/resources/TestData/ExcelFile.xlsx
@@ -1,41 +1,59 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eclise\selenuim\NopCommerceProject\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\janet\git\Uk-Project\ShopperStack_QUKN1\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87C053DD-914A-4688-86B6-575EF74E2820}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14916" windowHeight="6732"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Rakesh</t>
   </si>
   <si>
     <t>Rakesh@123</t>
   </si>
+  <si>
+    <t>Beauty</t>
+  </si>
+  <si>
+    <t>Mascara</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -357,11 +375,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -370,16 +388,21 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>